<commit_message>
TP with segment update MU multi OS and commands
</commit_message>
<xml_diff>
--- a/Specs et architecture/Cablage.xlsx
+++ b/Specs et architecture/Cablage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yves1812\Documents\GitHub\Robot_tondeuse\Specs et architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0174446-8F08-4586-B562-1FF9DD81D664}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE5B49F-FDAF-4E40-A2B5-64F50638B358}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16460" windowHeight="4960" xr2:uid="{E49B8D10-FDBE-40D4-9739-6103193CA538}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16460" windowHeight="4960" activeTab="4" xr2:uid="{E49B8D10-FDBE-40D4-9739-6103193CA538}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="95">
   <si>
     <t>DB pin</t>
   </si>
@@ -79,9 +79,6 @@
     <t>SS</t>
   </si>
   <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>Ground</t>
   </si>
   <si>
@@ -290,6 +287,39 @@
   </si>
   <si>
     <t>decode B (JST)</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>jaune</t>
+  </si>
+  <si>
+    <t>beige</t>
+  </si>
+  <si>
+    <t>ICSP</t>
+  </si>
+  <si>
+    <t>in 1</t>
+  </si>
+  <si>
+    <t>in 2</t>
+  </si>
+  <si>
+    <t>en 12</t>
+  </si>
+  <si>
+    <t>in 3</t>
+  </si>
+  <si>
+    <t>in 4</t>
+  </si>
+  <si>
+    <t>en 34</t>
   </si>
 </sst>
 </file>
@@ -305,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +372,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -355,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -366,12 +420,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF996633"/>
+      <color rgb="FFFF99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -682,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EC9AD7-5937-4E68-9FBA-8342A8F57B71}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
@@ -690,17 +754,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +777,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,102 +790,110 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1</v>
@@ -833,18 +905,18 @@
         <v>1</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="9">
         <v>20</v>
@@ -853,18 +925,18 @@
         <v>8</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="9">
         <v>21</v>
@@ -873,47 +945,47 @@
         <v>8</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +998,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,10 +1010,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -961,16 +1033,16 @@
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2">
         <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -981,16 +1053,16 @@
         <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2">
         <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1001,16 +1073,16 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2">
         <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1030,49 +1102,47 @@
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1082,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5E5C1B-2EC5-449B-888E-7C24D28A35C7}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1095,9 +1165,9 @@
     <col min="6" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1106,19 +1176,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1129,13 +1199,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1147,12 +1220,15 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1165,11 +1241,14 @@
       <c r="D4" s="2"/>
       <c r="E4" s="4"/>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1183,52 +1262,61 @@
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>23</v>
       </c>
       <c r="B8">
         <v>22</v>
@@ -1237,15 +1325,18 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>24</v>
@@ -1255,14 +1346,17 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -1273,13 +1367,16 @@
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>52</v>
@@ -1291,91 +1388,94 @@
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
       <c r="G11" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D14" s="2" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1385,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CCCCF8-576A-46D4-85AE-7E7C09EA4850}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1397,9 +1497,9 @@
     <col min="5" max="5" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1408,15 +1508,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -1425,28 +1525,34 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>31</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1455,43 +1561,52 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>33</v>
-      </c>
-      <c r="B6">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>34</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1500,43 +1615,52 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
         <v>36</v>
-      </c>
-      <c r="B9">
-        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1546,42 +1670,51 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
         <v>38</v>
-      </c>
-      <c r="B11">
-        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1591,95 +1724,104 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DB & TP to reflect new wiring
</commit_message>
<xml_diff>
--- a/Specs et architecture/Cablage.xlsx
+++ b/Specs et architecture/Cablage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yves1812\Documents\GitHub\Robot_tondeuse\Specs et architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EEE1B0-5699-4F36-898A-B794C75F3BE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2929A294-4485-480C-9E6E-047D002C569B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16460" windowHeight="4960" activeTab="5" xr2:uid="{E49B8D10-FDBE-40D4-9739-6103193CA538}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16460" windowHeight="4960" activeTab="4" xr2:uid="{E49B8D10-FDBE-40D4-9739-6103193CA538}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="4" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5E5C1B-2EC5-449B-888E-7C24D28A35C7}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1667,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CCCCF8-576A-46D4-85AE-7E7C09EA4850}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>